<commit_message>
Update: booleanConstants and unary
</commit_message>
<xml_diff>
--- a/LanguageSpecs/First and Follow Sets.xlsx
+++ b/LanguageSpecs/First and Follow Sets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/CodingProjects/GitHub/Compiler-Construction/LanguageSpecs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271BA4A9-900F-2244-8954-E2BADE8FB378}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE6BFE9-4A06-3A46-8032-58FAC3DD292D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{3FEBC4A9-0A37-F649-BEF0-00E8881A387D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="1" xr2:uid="{3FEBC4A9-0A37-F649-BEF0-00E8881A387D}"/>
   </bookViews>
   <sheets>
     <sheet name="FirstFollow" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="198">
   <si>
     <t>First Set</t>
   </si>
@@ -367,9 +367,6 @@
     <t>CASE, ε</t>
   </si>
   <si>
-    <t>NUM, true, false</t>
-  </si>
-  <si>
     <t>DEFAULT, ε</t>
   </si>
   <si>
@@ -388,13 +385,7 @@
     <t>As per mail</t>
   </si>
   <si>
-    <t>Accounting for negative expressions</t>
-  </si>
-  <si>
     <t>BO, ID, NUM, RNUM</t>
-  </si>
-  <si>
-    <t>ID, NUM, RNUM, true, false?</t>
   </si>
   <si>
     <r>
@@ -732,30 +723,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">GET_VALUE BO ID BC SEMICOL | PRINT BO </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="17"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;var&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="17"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>BC SEMICOL</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">ID </t>
     </r>
     <r>
@@ -1353,91 +1320,229 @@
     <t xml:space="preserve">&lt;ioStmt&gt;|&lt;simpleStmt&gt;|&lt;declareStmt&gt;|&lt;conditionalStmt&gt;|&lt;iterativeStmt&gt; </t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">&lt;arithmeticOrBooleanExpr&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="17"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">| MINUS BO </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="17"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;arithmeticExpr&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="17"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">BC | PLUS BO </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="17"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>&lt;arithmeticExpr&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="17"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> BC</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">ID &lt;whichId&gt; | NUM | RNUM </t>
   </si>
   <si>
-    <r>
-      <t>&lt;arithmeticExpr&gt; &lt;recTerm_again&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="17"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> | TRUE | FALSE</t>
-    </r>
-  </si>
-  <si>
     <t>BO, ID, NUM, RNUM, TRUE, FALSE</t>
   </si>
   <si>
     <t>MINUS, BO, ID, NUM, RNUM, PLUS, TRUE FALSE</t>
-  </si>
-  <si>
-    <t>SEMICOL, TRUE, FALSE</t>
   </si>
   <si>
     <t>FIRST set of terminals are trivial as the include themselves only. 
 For every terminal &lt;T&gt; FIRST(&lt;T&gt;)={T}</t>
   </si>
   <si>
-    <t>NUM | TRUE | FALSE</t>
+    <t>booleanConstants</t>
+  </si>
+  <si>
+    <t>TRUE | FALSE</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">NUM | </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>&lt;booleanConstants&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;arithmeticExpr&gt; &lt;recTerm_again&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="17"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> | </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>&lt;booleanConstants&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">GET_VALUE BO ID BC SEMICOL | PRINT BO </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;var&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="17"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">BC SEMICOL | PRINT BO </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>&lt;booleanConstants&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="17"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> BC SEMICOL</t>
+    </r>
+  </si>
+  <si>
+    <t>Defined Bool Consts</t>
+  </si>
+  <si>
+    <t>unary</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MINUS BO </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>&lt;arithmeticExpr&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="17"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> BC | PLUS BO </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>&lt;arithmeticExpr&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="17"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> BC | MINUS </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>&lt;var&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="17"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> | PLUS </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>&lt;var&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;arithmeticOrBooleanExpr&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="17"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">| </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>&lt;unary&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>MINUS | PLUS</t>
+  </si>
+  <si>
+    <t>TRUE, FALSE</t>
+  </si>
+  <si>
+    <t>BC, COLON, AND, OR, SEMICOL</t>
+  </si>
+  <si>
+    <t>NUM, TRUE, FAKSE</t>
+  </si>
+  <si>
+    <t>Bool Constants for print</t>
+  </si>
+  <si>
+    <t>Accounting for unary expressions</t>
+  </si>
+  <si>
+    <t>arithmeticOrBooleanExpr_again</t>
+  </si>
+  <si>
+    <t>arithmeticOrBooleanExpr</t>
   </si>
 </sst>
 </file>
@@ -1469,26 +1574,6 @@
       <b/>
       <sz val="17"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="20"/>
-      <color rgb="FF00B050"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="20"/>
-      <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -1545,6 +1630,26 @@
       <b/>
       <sz val="35"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF00B050"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -1669,7 +1774,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1680,67 +1785,70 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1749,26 +1857,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2086,24 +2194,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6822BB1F-EDCB-F342-A09E-E15946EFE70E}">
   <dimension ref="A1:C99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView view="pageLayout" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="45.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="48" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.5" style="1" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15"/>
+      <c r="A1" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:3" ht="34" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -2117,588 +2225,625 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="C3" s="9" t="s">
+      <c r="B3" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="48" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="71" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="71" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="8" t="s">
+      <c r="C21" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B32" s="15"/>
+      <c r="C32" s="16"/>
+    </row>
+    <row r="33" spans="1:3" ht="34" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="48" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="48" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="48" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="42" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="42" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="42" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="42" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="9" t="s">
+      <c r="C51" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C56" s="6" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="48" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="C15" s="9" t="s">
+    <row r="57" spans="1:3" ht="53" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C57" s="6" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="27" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="71" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="82" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="82" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="82" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="82" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="82" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="82" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="82" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="82" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="48" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B32" s="29" t="s">
-        <v>185</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="48" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="B33" s="29" t="s">
-        <v>184</v>
-      </c>
-      <c r="C33" s="9" t="s">
+    <row r="58" spans="1:3" ht="74" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C58" s="6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B34" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="48" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="B35" s="29" t="s">
-        <v>184</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="B36" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="42" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B37" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="42" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="B38" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="B39" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="B40" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B41" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="B42" s="29" t="s">
-        <v>120</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="42" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="82" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="82" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="82" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="30" t="s">
-        <v>187</v>
-      </c>
-      <c r="B55" s="31"/>
-      <c r="C55" s="32"/>
-    </row>
-    <row r="56" spans="1:3" ht="20" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="58" spans="1:3" ht="74" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" spans="1:3" ht="74" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="1:3" ht="74" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" spans="1:3" ht="74" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="B59" s="18"/>
+      <c r="C59" s="19"/>
+    </row>
+    <row r="60" spans="1:3" ht="74" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="61" spans="1:3" ht="74" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="62" spans="1:3" ht="74" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="63" spans="1:3" ht="74" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2739,11 +2884,16 @@
     <row r="98" ht="74" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="99" ht="74" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="A32:C32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="62" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <headerFooter>
+    <oddFooter>&amp;CPage 2 of 2</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2751,8 +2901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB0AD01-E814-8C4E-B795-59A92B7C67F0}">
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A34" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -2760,187 +2910,187 @@
     <col min="1" max="1" width="5.5" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" style="3" customWidth="1"/>
-    <col min="4" max="4" width="140.5" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17" style="3" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="146.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" style="3" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="86" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="21"/>
-    </row>
-    <row r="2" spans="1:6" ht="46" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+    <row r="1" spans="1:6" ht="85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="22"/>
+    </row>
+    <row r="2" spans="1:6" ht="50" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="24"/>
-    </row>
-    <row r="3" spans="1:6" ht="66" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="25"/>
+    </row>
+    <row r="3" spans="1:6" ht="54" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="26"/>
+      <c r="C3" s="27"/>
       <c r="D3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="11" t="s">
+      <c r="C4" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="C5" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="C6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>4</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="C7" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>5</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="E8" s="7" t="s">
+      <c r="C8" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="30" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>6</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="E9" s="5" t="s">
+      <c r="C9" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E9" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>7</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="E10" s="5" t="s">
+      <c r="C10" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E10" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="29" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2948,19 +3098,19 @@
       <c r="A11" s="4">
         <v>8</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="E11" s="16" t="s">
+      <c r="C11" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E11" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="31" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2968,35 +3118,35 @@
       <c r="A12" s="4">
         <v>9</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
+      <c r="C12" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
     </row>
     <row r="13" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>10</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="E13" s="16" t="s">
+      <c r="C13" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E13" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="31" t="s">
         <v>65</v>
       </c>
     </row>
@@ -3004,796 +3154,861 @@
       <c r="A14" s="4">
         <v>11</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-    </row>
-    <row r="15" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+    </row>
+    <row r="15" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>12</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="E15" s="5" t="s">
+      <c r="C15" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E15" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>13</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="8" t="s">
+      <c r="C16" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>14</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="E17" s="5" t="s">
+      <c r="C17" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E17" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>15</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="E18" s="5" t="s">
+      <c r="C18" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E18" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>16</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="E19" s="5" t="s">
+      <c r="C19" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="E19" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="52" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>17</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="30" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>18</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="8" t="s">
+      <c r="C21" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>19</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="11" t="s">
+      <c r="C22" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>20</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="E23" s="5" t="s">
+      <c r="C23" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E23" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>21</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="11" t="s">
+      <c r="C24" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>22</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="E25" s="5" t="s">
+      <c r="C25" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E25" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>23</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="E26" s="5" t="s">
+      <c r="C26" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="E26" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>24</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" s="8" t="s">
+      <c r="C27" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>25</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="E28" s="5" t="s">
+      <c r="C28" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E28" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="F28" s="29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>26</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="E29" s="5" t="s">
+      <c r="C29" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="E29" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="F29" s="29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+    <row r="30" spans="1:6" ht="79" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="22"/>
+    </row>
+    <row r="31" spans="1:6" ht="54" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="27"/>
+      <c r="D31" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
         <v>27</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B32" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="E30" s="16" t="s">
+      <c r="C32" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E32" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="F30" s="16" t="s">
+      <c r="F32" s="31" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
-        <v>28</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-    </row>
-    <row r="32" spans="1:6" ht="80" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
-        <v>29</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D32" s="33" t="s">
-        <v>181</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
+        <v>28</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+    </row>
+    <row r="34" spans="1:6" ht="59" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>29</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F34" s="30" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
         <v>30</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B35" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="E35" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F35" s="33" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>31</v>
+      </c>
+      <c r="B36" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D33" s="11" t="s">
+      <c r="C36" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="E36" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="F33" s="16" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
-        <v>31</v>
-      </c>
-      <c r="B34" s="10" t="s">
+      <c r="F36" s="31" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>32</v>
+      </c>
+      <c r="B37" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C34" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-    </row>
-    <row r="35" spans="1:6" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
-        <v>32</v>
-      </c>
-      <c r="B35" s="10" t="s">
+      <c r="C37" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
+    </row>
+    <row r="38" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>33</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C35" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-    </row>
-    <row r="36" spans="1:6" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
-        <v>33</v>
-      </c>
-      <c r="B36" s="10" t="s">
+      <c r="C38" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
+    </row>
+    <row r="39" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>34</v>
+      </c>
+      <c r="B39" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-    </row>
-    <row r="37" spans="1:6" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
-        <v>34</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="E37" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="F37" s="16" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="47" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
-        <v>35</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-    </row>
-    <row r="39" spans="1:6" ht="40" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
-        <v>36</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="F39" s="16" t="s">
-        <v>65</v>
-      </c>
+      <c r="C39" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="E39" s="32"/>
+      <c r="F39" s="32"/>
     </row>
     <row r="40" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
+        <v>35</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E40" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F40" s="31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>36</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="E41" s="32"/>
+      <c r="F41" s="32"/>
+    </row>
+    <row r="42" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
         <v>37</v>
       </c>
-      <c r="B40" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-    </row>
-    <row r="41" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
-        <v>38</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="54" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
-        <v>39</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D42" s="29" t="s">
-        <v>182</v>
-      </c>
-      <c r="E42" s="7" t="s">
+      <c r="B42" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E42" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="F42" s="7" t="s">
-        <v>85</v>
+      <c r="F42" s="31" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
-        <v>40</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C43" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="E43" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="F43" s="16" t="s">
-        <v>81</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="E43" s="32"/>
+      <c r="F43" s="32"/>
     </row>
     <row r="44" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
+        <v>39</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="E44" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="F44" s="29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="40" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>40</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E45" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F45" s="30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="40" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
         <v>41</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B46" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="E46" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="F46" s="33" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>42</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E47" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F47" s="31" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>43</v>
+      </c>
+      <c r="B48" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C44" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D44" s="8" t="s">
+      <c r="C48" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D48" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
-    </row>
-    <row r="45" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
-        <v>42</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
-        <v>43</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="C46" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="28" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
-        <v>44</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="28" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
-        <v>45</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C48" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>66</v>
-      </c>
+      <c r="E48" s="32"/>
+      <c r="F48" s="32"/>
     </row>
     <row r="49" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
-        <v>46</v>
-      </c>
-      <c r="B49" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C49" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="E49" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="F49" s="16" t="s">
-        <v>84</v>
+        <v>44</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E49" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="F49" s="29" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
+        <v>45</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E50" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="F50" s="29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>46</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E51" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="F51" s="29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
         <v>47</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="B52" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E52" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="F52" s="29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>48</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E53" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F53" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <v>49</v>
+      </c>
+      <c r="B54" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C50" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
-    </row>
-    <row r="51" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="4">
-        <v>48</v>
-      </c>
-      <c r="B51" s="10" t="s">
+      <c r="C54" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E54" s="32"/>
+      <c r="F54" s="32"/>
+    </row>
+    <row r="55" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <v>50</v>
+      </c>
+      <c r="B55" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C51" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D51" s="29" t="s">
-        <v>188</v>
-      </c>
-      <c r="E51" s="5" t="s">
+      <c r="C55" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="E55" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F51" s="6" t="s">
+      <c r="F55" s="29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="4">
-        <v>49</v>
-      </c>
-      <c r="B52" s="10" t="s">
+    <row r="56" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
+        <v>51</v>
+      </c>
+      <c r="B56" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C52" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="E52" s="5" t="s">
+      <c r="C56" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="E56" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F52" s="6" t="s">
+      <c r="F56" s="29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="48" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="4">
-        <v>50</v>
-      </c>
-      <c r="B53" s="10" t="s">
+    <row r="57" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
+        <v>52</v>
+      </c>
+      <c r="B57" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C53" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="E53" s="5" t="s">
+      <c r="C57" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E57" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F53" s="6" t="s">
+      <c r="F57" s="29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="4">
-        <v>51</v>
-      </c>
-      <c r="B54" s="10" t="s">
+    <row r="58" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
+        <v>53</v>
+      </c>
+      <c r="B58" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C54" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D54" s="8" t="s">
+      <c r="C58" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D58" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E54" s="5" t="s">
+      <c r="E58" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F54" s="6" t="s">
+      <c r="F58" s="29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="20" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F56" s="1"/>
-    </row>
-    <row r="58" spans="1:6" ht="74" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" spans="1:6" ht="74" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="1:6" ht="74" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" spans="1:6" ht="74" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+    </row>
+    <row r="60" spans="1:6" ht="74" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F60" s="1"/>
+    </row>
     <row r="61" spans="1:6" ht="74" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="62" spans="1:6" ht="74" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="63" spans="1:6" ht="74" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3835,28 +4050,33 @@
     <row r="99" ht="74" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="100" ht="74" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="21">
+    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="E36:E39"/>
+    <mergeCell ref="F36:F39"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="F42:F43"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="F13:F14"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="E33:E36"/>
-    <mergeCell ref="F33:F36"/>
   </mergeCells>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="53" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <headerFooter>
+    <oddFooter>&amp;CPage 2 of 2</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>